<commit_message>
Generated income distribution files for three data sets in excel
</commit_message>
<xml_diff>
--- a/Scripts_vjcortesa/data_output/Income_dist_housinggame_session_20_251007_VerzekeraarsMasterClass.xlsx
+++ b/Scripts_vjcortesa/data_output/Income_dist_housinggame_session_20_251007_VerzekeraarsMasterClass.xlsx
@@ -360,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T121"/>
+  <dimension ref="A1:S121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,11 +462,6 @@
           <t>calculated_spendable</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>calculated_difference_spendable</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -528,9 +523,6 @@
       <c r="S2">
         <v>5000</v>
       </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -592,9 +584,6 @@
       <c r="S3">
         <v>2000</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -656,9 +645,6 @@
       <c r="S4">
         <v>2500</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -720,9 +706,6 @@
       <c r="S5">
         <v>1750</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -784,9 +767,6 @@
       <c r="S6">
         <v>-3250</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -848,9 +828,6 @@
       <c r="S7">
         <v>30000</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -912,9 +889,6 @@
       <c r="S8">
         <v>7000</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -976,9 +950,6 @@
       <c r="S9">
         <v>2000</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -1040,9 +1011,6 @@
       <c r="S10">
         <v>1000</v>
       </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -1104,9 +1072,6 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -1168,9 +1133,6 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -1232,9 +1194,6 @@
       <c r="S13">
         <v>-7400</v>
       </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -1296,9 +1255,6 @@
       <c r="S14">
         <v>-4400</v>
       </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -1360,9 +1316,6 @@
       <c r="S15">
         <v>-5400</v>
       </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -1424,9 +1377,6 @@
       <c r="S16">
         <v>28100</v>
       </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -1488,9 +1438,6 @@
       <c r="S17">
         <v>15000</v>
       </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -1552,9 +1499,6 @@
       <c r="S18">
         <v>7000</v>
       </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -1616,9 +1560,6 @@
       <c r="S19">
         <v>10500</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -1680,9 +1621,6 @@
       <c r="S20">
         <v>16500</v>
       </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1744,9 +1682,6 @@
       <c r="S21">
         <v>18400</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -1808,9 +1743,6 @@
       <c r="S22">
         <v>50000</v>
       </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1872,9 +1804,6 @@
       <c r="S23">
         <v>37750</v>
       </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -1936,9 +1865,6 @@
       <c r="S24">
         <v>35000</v>
       </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -2000,9 +1926,6 @@
       <c r="S25">
         <v>39125</v>
       </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -2064,9 +1987,6 @@
       <c r="S26">
         <v>43250</v>
       </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -2128,9 +2048,6 @@
       <c r="S27">
         <v>80000</v>
       </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -2192,9 +2109,6 @@
       <c r="S28">
         <v>85500</v>
       </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -2256,9 +2170,6 @@
       <c r="S29">
         <v>79000</v>
       </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -2320,9 +2231,6 @@
       <c r="S30">
         <v>94500</v>
       </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -2384,9 +2292,6 @@
       <c r="S31">
         <v>8625</v>
       </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -2448,9 +2353,6 @@
       <c r="S32">
         <v>5000</v>
       </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -2512,9 +2414,6 @@
       <c r="S33">
         <v>7400</v>
       </c>
-      <c r="T33">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -2576,9 +2475,6 @@
       <c r="S34">
         <v>-200</v>
       </c>
-      <c r="T34">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -2640,9 +2536,6 @@
       <c r="S35">
         <v>200</v>
       </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -2704,9 +2597,6 @@
       <c r="S36">
         <v>200</v>
       </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -2768,9 +2658,6 @@
       <c r="S37">
         <v>30000</v>
       </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -2832,9 +2719,6 @@
       <c r="S38">
         <v>6000</v>
       </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -2896,9 +2780,6 @@
       <c r="S39">
         <v>7000</v>
       </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -2960,9 +2841,6 @@
       <c r="S40">
         <v>2000</v>
       </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -3024,9 +2902,6 @@
       <c r="S41">
         <v>0</v>
       </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -3088,9 +2963,6 @@
       <c r="S42">
         <v>0</v>
       </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -3152,9 +3024,6 @@
       <c r="S43">
         <v>1250</v>
       </c>
-      <c r="T43">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -3216,9 +3085,6 @@
       <c r="S44">
         <v>-15250</v>
       </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -3280,9 +3146,6 @@
       <c r="S45">
         <v>-16250</v>
       </c>
-      <c r="T45">
-        <v>0</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -3344,9 +3207,6 @@
       <c r="S46">
         <v>-17250</v>
       </c>
-      <c r="T46">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -3408,9 +3268,6 @@
       <c r="S47">
         <v>15000</v>
       </c>
-      <c r="T47">
-        <v>0</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -3472,9 +3329,6 @@
       <c r="S48">
         <v>-3000</v>
       </c>
-      <c r="T48">
-        <v>0</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -3536,9 +3390,6 @@
       <c r="S49">
         <v>-2700</v>
       </c>
-      <c r="T49">
-        <v>0</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -3600,9 +3451,6 @@
       <c r="S50">
         <v>5300</v>
       </c>
-      <c r="T50">
-        <v>0</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -3664,9 +3512,6 @@
       <c r="S51">
         <v>38300</v>
       </c>
-      <c r="T51">
-        <v>0</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -3728,9 +3573,6 @@
       <c r="S52">
         <v>50000</v>
       </c>
-      <c r="T52">
-        <v>0</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -3792,9 +3634,6 @@
       <c r="S53">
         <v>42000</v>
       </c>
-      <c r="T53">
-        <v>0</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -3856,9 +3695,6 @@
       <c r="S54">
         <v>19000</v>
       </c>
-      <c r="T54">
-        <v>0</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -3920,9 +3756,6 @@
       <c r="S55">
         <v>8500</v>
       </c>
-      <c r="T55">
-        <v>0</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -3984,9 +3817,6 @@
       <c r="S56">
         <v>4500</v>
       </c>
-      <c r="T56">
-        <v>0</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -4048,9 +3878,6 @@
       <c r="S57">
         <v>80000</v>
       </c>
-      <c r="T57">
-        <v>0</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -4112,9 +3939,6 @@
       <c r="S58">
         <v>65500</v>
       </c>
-      <c r="T58">
-        <v>0</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -4176,9 +4000,6 @@
       <c r="S59">
         <v>76000</v>
       </c>
-      <c r="T59">
-        <v>0</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -4240,9 +4061,6 @@
       <c r="S60">
         <v>56500</v>
       </c>
-      <c r="T60">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -4304,9 +4122,6 @@
       <c r="S61">
         <v>43500</v>
       </c>
-      <c r="T61">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -4368,9 +4183,6 @@
       <c r="S62">
         <v>5000</v>
       </c>
-      <c r="T62">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -4432,9 +4244,6 @@
       <c r="S63">
         <v>10000</v>
       </c>
-      <c r="T63">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -4496,9 +4305,6 @@
       <c r="S64">
         <v>11000</v>
       </c>
-      <c r="T64">
-        <v>0</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -4560,9 +4366,6 @@
       <c r="S65">
         <v>3000</v>
       </c>
-      <c r="T65">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -4624,9 +4427,6 @@
       <c r="S66">
         <v>500</v>
       </c>
-      <c r="T66">
-        <v>0</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -4688,9 +4488,6 @@
       <c r="S67">
         <v>30000</v>
       </c>
-      <c r="T67">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -4752,9 +4549,6 @@
       <c r="S68">
         <v>16125</v>
       </c>
-      <c r="T68">
-        <v>0</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -4816,9 +4610,6 @@
       <c r="S69">
         <v>13875</v>
       </c>
-      <c r="T69">
-        <v>0</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -4880,9 +4671,6 @@
       <c r="S70">
         <v>14000</v>
       </c>
-      <c r="T70">
-        <v>0</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -4944,9 +4732,6 @@
       <c r="S71">
         <v>14125</v>
       </c>
-      <c r="T71">
-        <v>0</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -5008,9 +4793,6 @@
       <c r="S72">
         <v>0</v>
       </c>
-      <c r="T72">
-        <v>0</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -5072,9 +4854,6 @@
       <c r="S73">
         <v>600</v>
       </c>
-      <c r="T73">
-        <v>0</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -5136,9 +4915,6 @@
       <c r="S74">
         <v>450</v>
       </c>
-      <c r="T74">
-        <v>0</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -5200,9 +4976,6 @@
       <c r="S75">
         <v>-3700</v>
       </c>
-      <c r="T75">
-        <v>0</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -5264,9 +5037,6 @@
       <c r="S76">
         <v>700</v>
       </c>
-      <c r="T76">
-        <v>0</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -5328,9 +5098,6 @@
       <c r="S77">
         <v>15000</v>
       </c>
-      <c r="T77">
-        <v>0</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -5392,9 +5159,6 @@
       <c r="S78">
         <v>-8000</v>
       </c>
-      <c r="T78">
-        <v>0</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -5456,9 +5220,6 @@
       <c r="S79">
         <v>-5000</v>
       </c>
-      <c r="T79">
-        <v>0</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -5520,9 +5281,6 @@
       <c r="S80">
         <v>-2000</v>
       </c>
-      <c r="T80">
-        <v>0</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -5584,9 +5342,6 @@
       <c r="S81">
         <v>1000</v>
       </c>
-      <c r="T81">
-        <v>0</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -5648,9 +5403,6 @@
       <c r="S82">
         <v>50000</v>
       </c>
-      <c r="T82">
-        <v>0</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -5712,9 +5464,6 @@
       <c r="S83">
         <v>42500</v>
       </c>
-      <c r="T83">
-        <v>0</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -5776,9 +5525,6 @@
       <c r="S84">
         <v>37000</v>
       </c>
-      <c r="T84">
-        <v>0</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -5840,9 +5586,6 @@
       <c r="S85">
         <v>15500</v>
       </c>
-      <c r="T85">
-        <v>0</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -5904,9 +5647,6 @@
       <c r="S86">
         <v>5000</v>
       </c>
-      <c r="T86">
-        <v>0</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -5968,9 +5708,6 @@
       <c r="S87">
         <v>80000</v>
       </c>
-      <c r="T87">
-        <v>0</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -6032,9 +5769,6 @@
       <c r="S88">
         <v>93000</v>
       </c>
-      <c r="T88">
-        <v>0</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -6096,9 +5830,6 @@
       <c r="S89">
         <v>104000</v>
       </c>
-      <c r="T89">
-        <v>0</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -6160,9 +5891,6 @@
       <c r="S90">
         <v>115500</v>
       </c>
-      <c r="T90">
-        <v>0</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -6224,9 +5952,6 @@
       <c r="S91">
         <v>122000</v>
       </c>
-      <c r="T91">
-        <v>0</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -6288,9 +6013,6 @@
       <c r="S92">
         <v>5000</v>
       </c>
-      <c r="T92">
-        <v>0</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -6352,9 +6074,6 @@
       <c r="S93">
         <v>-9000</v>
       </c>
-      <c r="T93">
-        <v>0</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -6416,9 +6135,6 @@
       <c r="S94">
         <v>-4000</v>
       </c>
-      <c r="T94">
-        <v>0</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -6480,9 +6196,6 @@
       <c r="S95">
         <v>-10125</v>
       </c>
-      <c r="T95">
-        <v>0</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -6544,9 +6257,6 @@
       <c r="S96">
         <v>-1125</v>
       </c>
-      <c r="T96">
-        <v>0</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -6608,9 +6318,6 @@
       <c r="S97">
         <v>30000</v>
       </c>
-      <c r="T97">
-        <v>0</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -6672,9 +6379,6 @@
       <c r="S98">
         <v>26000</v>
       </c>
-      <c r="T98">
-        <v>0</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -6736,9 +6440,6 @@
       <c r="S99">
         <v>22300</v>
       </c>
-      <c r="T99">
-        <v>0</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -6800,9 +6501,6 @@
       <c r="S100">
         <v>3600</v>
       </c>
-      <c r="T100">
-        <v>0</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -6864,9 +6562,6 @@
       <c r="S101">
         <v>6400</v>
       </c>
-      <c r="T101">
-        <v>0</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -6928,9 +6623,6 @@
       <c r="S102">
         <v>0</v>
       </c>
-      <c r="T102">
-        <v>0</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -6992,9 +6684,6 @@
       <c r="S103">
         <v>1600</v>
       </c>
-      <c r="T103">
-        <v>0</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -7056,9 +6745,6 @@
       <c r="S104">
         <v>200</v>
       </c>
-      <c r="T104">
-        <v>0</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -7120,9 +6806,6 @@
       <c r="S105">
         <v>800</v>
       </c>
-      <c r="T105">
-        <v>0</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -7184,9 +6867,6 @@
       <c r="S106">
         <v>800</v>
       </c>
-      <c r="T106">
-        <v>0</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -7248,9 +6928,6 @@
       <c r="S107">
         <v>15000</v>
       </c>
-      <c r="T107">
-        <v>0</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -7312,9 +6989,6 @@
       <c r="S108">
         <v>10000</v>
       </c>
-      <c r="T108">
-        <v>0</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -7376,9 +7050,6 @@
       <c r="S109">
         <v>4250</v>
       </c>
-      <c r="T109">
-        <v>0</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -7440,9 +7111,6 @@
       <c r="S110">
         <v>11100</v>
       </c>
-      <c r="T110">
-        <v>0</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -7504,9 +7172,6 @@
       <c r="S111">
         <v>17950</v>
       </c>
-      <c r="T111">
-        <v>0</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -7568,9 +7233,6 @@
       <c r="S112">
         <v>50000</v>
       </c>
-      <c r="T112">
-        <v>0</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -7632,9 +7294,6 @@
       <c r="S113">
         <v>66000</v>
       </c>
-      <c r="T113">
-        <v>0</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -7696,9 +7355,6 @@
       <c r="S114">
         <v>65500</v>
       </c>
-      <c r="T114">
-        <v>0</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -7760,9 +7416,6 @@
       <c r="S115">
         <v>59500</v>
       </c>
-      <c r="T115">
-        <v>0</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -7824,9 +7477,6 @@
       <c r="S116">
         <v>63500</v>
       </c>
-      <c r="T116">
-        <v>0</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -7888,9 +7538,6 @@
       <c r="S117">
         <v>80000</v>
       </c>
-      <c r="T117">
-        <v>0</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -7952,9 +7599,6 @@
       <c r="S118">
         <v>97800</v>
       </c>
-      <c r="T118">
-        <v>0</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -8016,9 +7660,6 @@
       <c r="S119">
         <v>112100</v>
       </c>
-      <c r="T119">
-        <v>0</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -8080,9 +7721,6 @@
       <c r="S120">
         <v>125900</v>
       </c>
-      <c r="T120">
-        <v>0</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -8143,9 +7781,6 @@
       </c>
       <c r="S121">
         <v>132200</v>
-      </c>
-      <c r="T121">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>